<commit_message>
more pics and data
</commit_message>
<xml_diff>
--- a/saint_peters/alt_stats.xlsx
+++ b/saint_peters/alt_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitch\Documents\GitHub\funsies\saint_peters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDFD036-EF06-49F1-AC03-5EF3C5FAA9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E69A7B-F244-4939-9D20-A92DE6170E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7818C230-33D9-4FA4-A813-139222D25B19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7818C230-33D9-4FA4-A813-139222D25B19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,42 +35,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>pace</t>
-  </si>
-  <si>
-    <t>efg</t>
-  </si>
-  <si>
-    <t>tov</t>
-  </si>
-  <si>
-    <t>orb</t>
-  </si>
-  <si>
     <t>ortg</t>
   </si>
   <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t>Murray State</t>
-  </si>
-  <si>
-    <t>Purdue</t>
-  </si>
-  <si>
     <t>Saint Peter's</t>
   </si>
   <si>
     <t>school</t>
   </si>
   <si>
-    <t>ft_fga</t>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Miami (FL)</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Villanova</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>Duke</t>
   </si>
 </sst>
 </file>
@@ -423,197 +420,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E66B34A-4446-4316-AEAB-338650BB9D55}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44637</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>68.7</v>
-      </c>
-      <c r="D2">
-        <v>0.58799999999999997</v>
-      </c>
-      <c r="E2">
-        <v>18.5</v>
-      </c>
-      <c r="F2">
-        <v>18.5</v>
-      </c>
-      <c r="G2">
-        <v>0.316</v>
-      </c>
-      <c r="H2">
         <v>110.4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
+        <v>44639</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>107.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>44645</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>101.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>44637</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>68.7</v>
-      </c>
-      <c r="D3">
-        <v>0.45900000000000002</v>
-      </c>
-      <c r="E3">
-        <v>13.6</v>
-      </c>
-      <c r="F3">
-        <v>31.6</v>
-      </c>
-      <c r="G3">
-        <v>0.377</v>
-      </c>
-      <c r="H3">
-        <v>102.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>121.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>44639</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>65.3</v>
-      </c>
-      <c r="D4">
-        <v>0.443</v>
-      </c>
-      <c r="E4">
-        <v>11.9</v>
-      </c>
-      <c r="F4">
-        <v>38.5</v>
-      </c>
-      <c r="G4">
-        <v>0.434</v>
-      </c>
-      <c r="H4">
-        <v>107.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>44639</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>65.3</v>
-      </c>
-      <c r="D5">
-        <v>0.42299999999999999</v>
-      </c>
-      <c r="E5">
-        <v>14.9</v>
-      </c>
-      <c r="F5">
-        <v>30.6</v>
-      </c>
-      <c r="G5">
-        <v>0.308</v>
-      </c>
-      <c r="H5">
-        <v>92.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>44645</v>
-      </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>65.599999999999994</v>
-      </c>
-      <c r="D6">
-        <v>0.44400000000000001</v>
-      </c>
-      <c r="E6">
-        <v>11.2</v>
-      </c>
-      <c r="F6">
-        <v>18.8</v>
-      </c>
-      <c r="G6">
-        <v>0.35199999999999998</v>
-      </c>
-      <c r="H6">
-        <v>101.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>105.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44645</v>
       </c>
       <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44637</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>110.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44639</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>112.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44645</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>90.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44638</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44640</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>105.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44645</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44638</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>124.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44640</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>107.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44644</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44638</v>
+      </c>
+      <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
-        <v>65.599999999999994</v>
-      </c>
-      <c r="D7">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="E7">
-        <v>18.8</v>
-      </c>
-      <c r="F7">
-        <v>41.7</v>
-      </c>
-      <c r="G7">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="H7">
-        <v>97</v>
+      <c r="C17">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44640</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>116.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44644</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>44637</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>111.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>44639</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>74.599999999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>44644</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>93.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>44638</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>44640</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>126.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>44644</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>114.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>